<commit_message>
replace atan by asin
</commit_message>
<xml_diff>
--- a/ProjectPlan/ToDoList.xlsx
+++ b/ProjectPlan/ToDoList.xlsx
@@ -20,6 +20,36 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Auteur</author>
+  </authors>
+  <commentList>
+    <comment ref="B22" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">5 Mètres Chaine Simple-ISO standard Au pas de : 6 (6 x 2,8 mm)  04-B1 1
+Pignon Simple Pas 6 mm (04 1) Nbr de dents :9  PS04B09 2
+Pignon Simple Pas 6 mm (04 1) Nbr de dents :10  PS04B10 2
+Pignon Simple Pas 6 mm (04 1) Nbr de dents :12  PS04B12 2
+Attache rapide pour chaine : 04B1 6 x 2,8 mm  AR04B1 6
+Pignon Simple Pas 6 mm (04 1) Nbr de dents :8  PS04B08 2
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="92">
   <si>
@@ -246,9 +276,6 @@
     <t>1m used over 5m ordered</t>
   </si>
   <si>
-    <t>pinion</t>
-  </si>
-  <si>
     <t>transmission</t>
   </si>
   <si>
@@ -298,6 +325,9 @@
   </si>
   <si>
     <t>no fixed point</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pignions </t>
   </si>
 </sst>
 </file>
@@ -307,7 +337,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -330,6 +360,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -933,11 +970,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:O31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M32" sqref="M32"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -946,7 +983,7 @@
     <col min="2" max="2" width="63.85546875" customWidth="1"/>
     <col min="3" max="3" width="20.7109375" customWidth="1"/>
     <col min="4" max="4" width="7.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" style="3" customWidth="1"/>
     <col min="7" max="7" width="7" style="11" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="4.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="7" style="3" bestFit="1" customWidth="1"/>
@@ -1050,7 +1087,7 @@
         <v>64</v>
       </c>
       <c r="C4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D4" s="10">
         <v>42291</v>
@@ -1088,10 +1125,10 @@
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D5" s="10">
         <v>42305</v>
@@ -1114,7 +1151,7 @@
         <v>1.57</v>
       </c>
       <c r="K5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="M5" t="s">
         <v>51</v>
@@ -1154,7 +1191,7 @@
         <v>42299</v>
       </c>
       <c r="K6" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="M6" t="s">
         <v>51</v>
@@ -1246,10 +1283,10 @@
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D9" s="10">
         <v>42274</v>
@@ -1275,7 +1312,7 @@
         <v>42299</v>
       </c>
       <c r="K9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="M9" t="s">
         <v>51</v>
@@ -1336,7 +1373,7 @@
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C11" t="s">
         <v>56</v>
@@ -1460,7 +1497,7 @@
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D14" s="10"/>
       <c r="E14" s="3" t="s">
@@ -1564,7 +1601,7 @@
         <v>68</v>
       </c>
       <c r="C17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I17" s="11">
         <f t="shared" si="0"/>
@@ -1631,7 +1668,7 @@
         <v>71</v>
       </c>
       <c r="C21" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D21" s="10">
         <v>42331</v>
@@ -1675,10 +1712,10 @@
     </row>
     <row r="22" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
+        <v>91</v>
+      </c>
+      <c r="C22" t="s">
         <v>74</v>
-      </c>
-      <c r="C22" t="s">
-        <v>75</v>
       </c>
       <c r="D22" s="10">
         <v>42332</v>
@@ -1718,10 +1755,10 @@
     </row>
     <row r="23" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
+        <v>83</v>
+      </c>
+      <c r="C23" t="s">
         <v>84</v>
-      </c>
-      <c r="C23" t="s">
-        <v>85</v>
       </c>
       <c r="D23" s="10">
         <v>42243</v>
@@ -1761,7 +1798,7 @@
     </row>
     <row r="24" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G24" s="11">
         <v>1</v>
@@ -1786,10 +1823,10 @@
     </row>
     <row r="25" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
+        <v>88</v>
+      </c>
+      <c r="C25" t="s">
         <v>89</v>
-      </c>
-      <c r="C25" t="s">
-        <v>90</v>
       </c>
       <c r="D25" s="10">
         <v>42245</v>
@@ -1817,7 +1854,7 @@
         <v>49</v>
       </c>
       <c r="L25" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="O25" s="7">
         <f t="shared" si="3"/>
@@ -1838,7 +1875,7 @@
     </row>
     <row r="28" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="O28" s="7">
         <f t="shared" si="3"/>
@@ -1861,6 +1898,7 @@
     <mergeCell ref="M1:O1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>